<commit_message>
updated experiment HC vs SA
</commit_message>
<xml_diff>
--- a/experiment/StateSpace.xlsx
+++ b/experiment/StateSpace.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marrit\Documents\School\2017-2018\Heuristieken\Proteins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amber\Documents\UvA\Master Jaar 2\Minor Programmeren\Programmeertheorie\Proteins\Proteins\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50257972-0834-49A1-A0E8-661B030CAA2D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0455F71B-CAC7-477D-8D41-EDD19633B202}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <t>?</t>
   </si>
   <si>
-    <t xml:space="preserve">bij 350000 keer prunen op -7 … </t>
+    <t xml:space="preserve">bij 77520000 keer prunen op -9 … </t>
   </si>
 </sst>
 </file>
@@ -741,6 +741,66 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,12 +810,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -763,60 +817,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1120,24 +1120,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3.5" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.69921875" customWidth="1"/>
-    <col min="8" max="8" width="18.69921875" style="5" customWidth="1"/>
-    <col min="9" max="23" width="10.796875" customWidth="1"/>
-    <col min="24" max="27" width="25.796875" customWidth="1"/>
-    <col min="28" max="28" width="20.796875" customWidth="1"/>
+    <col min="7" max="7" width="18.75" customWidth="1"/>
+    <col min="8" max="8" width="18.75" style="5" customWidth="1"/>
+    <col min="9" max="23" width="10.75" customWidth="1"/>
+    <col min="24" max="27" width="25.75" customWidth="1"/>
+    <col min="28" max="28" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="40.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>12</v>
       </c>
@@ -1153,50 +1153,50 @@
       <c r="E1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="70" t="s">
+      <c r="I1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="66"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="70" t="s">
+      <c r="M1" s="49"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="70" t="s">
+      <c r="P1" s="49"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="70" t="s">
+      <c r="S1" s="49"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="66"/>
-      <c r="W1" s="68"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="51"/>
     </row>
-    <row r="2" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55"/>
       <c r="B2" s="57"/>
       <c r="C2" s="59"/>
       <c r="D2" s="61"/>
       <c r="E2" s="63"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="69"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
@@ -1243,20 +1243,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="25.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="25.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="66">
         <v>8</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="67">
         <v>2</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="68">
         <v>6</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="64">
         <v>0</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1320,14 +1320,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1389,20 +1389,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="66">
         <v>14</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="67">
         <v>4</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="68">
         <v>10</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="64">
         <v>0</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1466,14 +1466,14 @@
         <v>2.7954578399658203E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="64"/>
       <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
@@ -1535,20 +1535,20 @@
         <v>2.8696484240489538E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>3</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="66">
         <v>20</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="67">
         <v>10</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="68">
         <v>10</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="64">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1612,14 +1612,14 @@
         <v>8.9785316959023476E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="64"/>
       <c r="F8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1675,20 +1675,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>4</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="66">
         <v>36</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="67">
         <v>20</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="68">
         <v>16</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="64">
         <v>0</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1743,19 +1743,19 @@
       <c r="V9" s="18">
         <v>40</v>
       </c>
-      <c r="W9" s="71">
+      <c r="W9" s="46">
         <f t="shared" si="4"/>
         <v>1.3552527156068805E-17</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>4</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="64"/>
       <c r="F10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1809,20 +1809,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>5</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="66">
         <v>50</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="67">
         <v>16</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="68">
         <v>24</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="64">
         <v>0</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1878,14 +1878,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>5</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="64"/>
       <c r="F12" s="6" t="s">
         <v>5</v>
       </c>
@@ -1939,20 +1939,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>6</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="66">
         <v>36</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="67">
         <v>18</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="68">
         <v>14</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E13" s="64">
         <v>4</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -2002,14 +2002,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>6</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="6" t="s">
         <v>5</v>
       </c>
@@ -2057,20 +2057,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>7</v>
       </c>
-      <c r="B15" s="46">
+      <c r="B15" s="66">
         <v>36</v>
       </c>
-      <c r="C15" s="47">
+      <c r="C15" s="67">
         <v>15</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="68">
         <v>11</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="64">
         <v>10</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -2120,14 +2120,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="6" t="s">
         <v>5</v>
       </c>
@@ -2175,20 +2175,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>8</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17" s="66">
         <v>50</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="67">
         <v>21</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="68">
         <v>19</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="64">
         <v>10</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -2238,14 +2238,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>8</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -2293,20 +2293,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>9</v>
       </c>
-      <c r="B19" s="46">
+      <c r="B19" s="66">
         <v>50</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="67">
         <v>23</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="68">
         <v>21</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="64">
         <v>6</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -2356,14 +2356,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>9</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="50"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="65"/>
       <c r="F20" s="14" t="s">
         <v>5</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="25.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1"/>
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
@@ -2425,7 +2425,7 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:23" ht="25.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I22" s="28"/>
       <c r="J22" t="s">
         <v>18</v>
@@ -2437,7 +2437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="25.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="25.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I23" s="27"/>
       <c r="J23" t="s">
         <v>19</v>
@@ -2447,38 +2447,35 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="29"/>
       <c r="J24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="B5:B6"/>
@@ -2495,21 +2492,24 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>